<commit_message>
Added new tests to suite file.
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData.xlsx
+++ b/src/test/resources/ExcelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Workspace\herokuapp-testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34633E06-C077-4262-B68D-F28F4272BCD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352CDF2A-F55D-4558-B579-45E67D24DA2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5873" yWindow="2753" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -207,9 +207,6 @@
     <t>name: user3</t>
   </si>
   <si>
-    <t>JavaScripAlertsExecution.testJavaScripAlerts</t>
-  </si>
-  <si>
     <t>I am a JS Alert</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>Incorrect row or column number</t>
+  </si>
+  <si>
+    <t>JavaScriptAlertsExecution.testJavaScriptAlerts</t>
   </si>
 </sst>
 </file>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -933,7 +933,7 @@
         <v>18</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">
@@ -1019,7 +1019,7 @@
         <v>21</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q4" s="2"/>
     </row>
@@ -1360,7 +1360,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="1"/>
@@ -1372,34 +1372,34 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1411,10 +1411,10 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1422,13 +1422,13 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1440,7 +1440,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1449,13 +1449,13 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1467,7 +1467,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="1"/>
@@ -1490,24 +1490,24 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="O22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="Q22" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="1"/>
@@ -1521,10 +1521,10 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="1"/>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>5</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>5</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="1"/>
@@ -1627,28 +1627,28 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="O27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="2"/>
     </row>
     <row r="28" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1658,10 +1658,10 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="N28" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>

</xml_diff>